<commit_message>
update report, log result
</commit_message>
<xml_diff>
--- a/data/testcases/testcases.xlsx
+++ b/data/testcases/testcases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,6 +11,8 @@
     <sheet name="Detail" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Cart" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Payment" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Demo" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Demo2" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -2665,7 +2667,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>safe_type() missing 1 required positional argument: 'text'</t>
+          <t>Thêm sản phẩm vào giỏ hàng thành công.</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -2850,7 +2852,7 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -3264,7 +3266,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Tổng tiền sản phẩm không hợp lệ</t>
+          <t>Tổng tiền sản phẩm là là hợp lệ</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -3306,12 +3308,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>list index out of range</t>
+          <t>"Tổng tiền giỏ hàng là hợp lệ, bằng tổng tiền các sản phẩm"</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -3506,13 +3508,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: 
-</t>
+          <t>"Chuyển hướng đến trang thanh toán"</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -4242,12 +4243,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Phương thức thanh toán lỗi vui lòng thử lại.</t>
+          <t>Chuyển hướng đến trang thanh toán MOMO</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -4284,12 +4285,1487 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Hiển thị thông báo bạn đã đặt hàng thành công</t>
+          <t>Không tìm thấy thông báo nào</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Loại test case</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Mô tả</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Dữ liệu test</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Kỳ vọng</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Thực tế</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Kết quả</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TC01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Kiểm tra sự hiển thị của ô tìm kiếm</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>"Ô tìm kiếm hiển thị, placeholder là 'Tìm kiếm sản phẩm'"</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ô tìm kiếm hiển thị placeholder là tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TC02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Kiểm tra sự hiển thị của button tìm kiếm</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>"Button tìm kiếm hiển thị"</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>button tìm kiếm hiển thị</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TC03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Kiểm tra placeholder của ô tìm kiếm</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>"Placeholder trong ô tìm kiếm là 'Tìm kiếm sản phẩm'"</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>placeholder trong ô tìm kiếm là tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TC04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Kiểm tra ngôn ngữ hiển thị của placeholder</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>"Placeholder hiển thị bằng tiếng Việt"</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>placeholder hiển thị bằng tiếng việt</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TC05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa có trong danh sách sản phẩm (Life)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Từ khóa: Life</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TC06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa không có trong danh sách sản phẩm (zzxy)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Từ khóa: zzxy</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm không hiển thị, button 'Xem thêm' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Không tìm được sản phẩm</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TC07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa có khoảng trắng ở đầu (  Life)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Từ khóa:   Life</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TC08</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa có khoảng trắng ở cuối (Life  )</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Từ khóa: Life</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TC09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa có cả khoảng trắng đầu và cuối (  Life  )</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Từ khóa:   Life</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TC10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa là chữ thường (life)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Từ khóa: life</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TC11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa là chữ hoa (LIFE)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Từ khóa: LIFE</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TC12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tìm kiếm bằng cách nhấn Enter</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Từ khóa: Life</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TC13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Tìm kiếm bằng cách nhấn nút tìm kiếm</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Từ khóa: Life</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm chứa 'Life' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TC14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa là ký tự đặc biệt (!@#)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Từ khóa: !@#</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm không hiển thị, button 'Xem thêm' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Hệ thống cho phép tìm kiếm với ký tự đặc biệt, có kết quả trả về</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TC15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa là số (12345)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Từ khóa: 12345</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm không hiển thị, button 'Xem thêm' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Hệ thống cho phép tìm kiếm với ký tự số, có kết quả trả về</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TC16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa là ký tự in hoa và số (LIFE123)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Từ khóa: LIFE123</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm không hiển thị, button 'Xem thêm' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Không tìm được sản phẩm</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TC17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Tìm kiếm sản phẩm</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tìm kiếm với từ khóa trống</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Từ khóa:</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm không hiển thị, button 'Xem thêm' hiển thị"</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>"Danh sách sản phẩm không hiển thị, button 'Xem thêm' hiển thị"</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Loại test case</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Mô tả</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Dữ liệu test</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Kỳ vọng</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Thực tế</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Kết quả</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TC01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Kiểm tra hiển thị các cột</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Hiển thị đầy đủ các cột: Sản Phẩm, Đơn giá, Số lượng, Tổng</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Không hỗ trợ mô tả</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Skip</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TC02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Kiểm tra ngôn ngữ hiển thị</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Ngôn ngữ hiển thị là tiếng Việt</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ngôn ngữ hiển thị là tiếng việt</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TC03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Kiểm tra hiển thị tổng tiền</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Hiển thị dòng tổng tiền</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>tổng tiền của giỏ hàng hiển thị đúng định dạng tiền tệ (vnđ) và giá trị chính xác (tổng của tất cả các tổng tiền sản phẩm)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TC04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Kiểm tra hiển thị button "Thanh toán"</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Hiển thị button "Thanh toán"</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>hiển thị button thanh toán</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TC05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Kiểm tra hiển thị liên kết "Tiếp tục mua sắm"</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Hiển thị liên kết "Tiếp tục mua sắm"</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>hiển thị liên kết tiếp tục mua sắm</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TC06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Kiểm tra hiển thị button xóa</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Hiển thị button xóa cho từng sản phẩm</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>hiển thị button xóa cho từng sản phẩm</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TC07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Kiểm tra tính toán tổng tiền khi số lượng sản phẩm là 2</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm 1: 2, Số lượng sản phẩm 2: 2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Tổng tiền hiển thị chính xác (tổng đơn giá * số lượng)</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Tổng tiền giỏ hàng là hợp lệ</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TC08</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Kiểm tra tính toán tổng của 1 sản phẩm</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm 1: 1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Tổng hiển thị chính xác bằng đơn giá</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm hợp lệ</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TC09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Kiểm tra thay đổi số lượng sản phẩm hợp lệ</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm 1: 2</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm được thay đổi thành công và tổng tiền được cập nhật tương ứng</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Tổng tiền giỏ hàng là hợp lệ</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TC10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Kiểm tra thay đổi số lượng sản phẩm nhỏ hơn 1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm 1: 0</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Hiển thị thông báo lỗi và số lượng không thay đổi</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>vẫn giảm về 0</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TC11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Kiểm tra thay đổi số lượng sản phẩm bằng 1</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm 1: 1</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm được thay đổi thành công</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm hợp lệ</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TC12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Kiểm tra thay đổi số lượng sản phẩm lớn hơn số lượng tồn kho</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Số lượng sản phẩm 1: 453</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Hiển thị thông báo lỗi và số lượng không thay đổi</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>vượt số lượng tồn kho</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TC13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Kiểm tra chức năng button "Thanh toán"</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Chuyển hướng đến trang thanh toán</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Chuyển hướng đến trang thanh toán</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TC14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Kiểm tra chức năng liên kết "Tiếp tục mua sắm"</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Chuyển hướng đến trang sản phẩm</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Chuyển hướng đến trang sản phẩm</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TC15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Kiểm tra chức năng button "Xóa"</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Sản phẩm được xóa khỏi giỏ hàng và cập nhật tổng tiền</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Sản phẩm bị xóa khỏi giỏ hàng thành công</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TC16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Kiểm tra xóa sản phẩm cuối cùng trong giỏ hàng</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Giỏ hàng trống, hiển thị thông báo (nếu có)</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Sản phẩm bị xóa khỏi giỏ hàng thành công</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TC17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Giỏ hàng</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Chức năng</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Kiểm tra tổng tiền khi giỏ hàng trống</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Tổng tiền hiển thị là 0</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Giỏ hàng không trống</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>

</xml_diff>